<commit_message>
chore: alteração nas colunas de telefone da tabela order_addresses
</commit_message>
<xml_diff>
--- a/resources/react-app/public/upload-file/template/Envio de endereços dos pedidos.xlsx
+++ b/resources/react-app/public/upload-file/template/Envio de endereços dos pedidos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Projetos\B1Sistema-PDOCRUD\resources\react-app\public\upload-file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE6198E-C9A4-43A8-AC7D-94EF26C772D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0D7F1-0CAB-47C7-9179-A691EF9F7012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4215F992-DD97-401D-9FF6-1FE2FD396920}"/>
+    <workbookView xWindow="-20610" yWindow="1710" windowWidth="20730" windowHeight="11160" xr2:uid="{4215F992-DD97-401D-9FF6-1FE2FD396920}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Nº Pedido</t>
   </si>
@@ -104,10 +104,58 @@
     <t>ship-country</t>
   </si>
   <si>
-    <t>Telefone</t>
-  </si>
-  <si>
-    <t>buyer-phone-number (tratar todos os números para não virem como 5,51E+12)</t>
+    <t>buyer-phone-number</t>
+  </si>
+  <si>
+    <t>Comprador</t>
+  </si>
+  <si>
+    <t>buyer-name</t>
+  </si>
+  <si>
+    <t>buyer-email</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Data Prevista</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Frete</t>
+  </si>
+  <si>
+    <t>Taxa do produto</t>
+  </si>
+  <si>
+    <t>Taxa do frete</t>
+  </si>
+  <si>
+    <t>latest-delivery-date</t>
+  </si>
+  <si>
+    <t>item-price - item-promotion-discount</t>
+  </si>
+  <si>
+    <t>shipping-price</t>
+  </si>
+  <si>
+    <t>item-tax</t>
+  </si>
+  <si>
+    <t>ship-tax</t>
+  </si>
+  <si>
+    <t>Telefone do comprador</t>
+  </si>
+  <si>
+    <t>Telefone do destinatário</t>
+  </si>
+  <si>
+    <t>ship-phone-number</t>
   </si>
 </sst>
 </file>
@@ -172,25 +220,25 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,216 +554,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01C4B1C-0ADB-497B-A762-48AAE86271F3}">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.90625" customWidth="1"/>
-    <col min="9" max="9" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" customWidth="1"/>
-    <col min="11" max="11" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.81640625" customWidth="1"/>
-    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="1.81640625" customWidth="1"/>
+    <col min="22" max="22" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="U2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="U4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
+      <c r="Y4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="U5" s="7"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>9</v>
-      </c>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="U6" s="7"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
     </row>
-    <row r="4" spans="1:24" s="5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="6"/>
-      <c r="M4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M5" s="7"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M6" s="7"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M7" s="7"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="U7" s="7"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="21">
+    <mergeCell ref="U2:AN2"/>
+    <mergeCell ref="X4:X7"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="V4:V7"/>
     <mergeCell ref="W4:W7"/>
-    <mergeCell ref="X4:X7"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="AB4:AB7"/>
+    <mergeCell ref="AC4:AC7"/>
+    <mergeCell ref="Z4:Z7"/>
+    <mergeCell ref="AA4:AA7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="AG4:AG7"/>
+    <mergeCell ref="AH4:AH7"/>
+    <mergeCell ref="AI4:AI7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="AD4:AD7"/>
+    <mergeCell ref="AE4:AE7"/>
+    <mergeCell ref="AJ4:AJ7"/>
+    <mergeCell ref="AK4:AK7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>